<commit_message>
docker flask port modify
</commit_message>
<xml_diff>
--- a/DOC/1. 개발 문서/개발현황.xlsx
+++ b/DOC/1. 개발 문서/개발현황.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minu0\바탕 화면\MDBS\DOC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minu0\바탕 화면\MDBS\DOC\1. 개발 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718B188E-3A51-40A9-B435-087C2673832F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E956145F-148B-4FFE-AD8B-F37E0F086947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E0CAA267-4327-4047-9EC4-6CAD6A2DA8A6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
   <si>
     <t xml:space="preserve">분류 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -206,6 +206,15 @@
   </si>
   <si>
     <t>2026 09 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mongo는 프로시저가 없어
+Flask에서 설정</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2026 09 26</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -385,7 +394,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -446,6 +455,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -809,7 +821,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9:I10"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -984,7 +996,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -998,7 +1010,9 @@
         <v>42</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
+      <c r="I9" s="17" t="s">
+        <v>44</v>
+      </c>
       <c r="J9" s="4"/>
       <c r="K9" s="5" t="s">
         <v>41</v>
@@ -1007,35 +1021,39 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E10" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="5"/>
-      <c r="L10" s="8"/>
+      <c r="K10" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E11" s="12" t="b">
         <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
       <c r="K11" s="5"/>
-      <c r="L11" s="8"/>
+      <c r="L11" s="5"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E12" s="12" t="b">

</xml_diff>

<commit_message>
procedure 연결 관련 file 수정
</commit_message>
<xml_diff>
--- a/DOC/1. 개발 문서/개발현황.xlsx
+++ b/DOC/1. 개발 문서/개발현황.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minu0\바탕 화면\MDBS\DOC\1. 개발 문서\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E956145F-148B-4FFE-AD8B-F37E0F086947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70BD25FB-8674-4074-B61F-1022A43F441C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{E0CAA267-4327-4047-9EC4-6CAD6A2DA8A6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="47">
   <si>
     <t xml:space="preserve">분류 </t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -153,10 +153,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2026 09 11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>2025 09 11</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -165,47 +161,15 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>데이터 바인딩</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Docker Flask 세팅</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DBMS에 성능 수치화</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SSE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SQL, Procedure</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RDG 프로그래밍</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2026 09 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>계좌 데이터 삽입</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2026 09 19</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>각 DB 송금 프로세스(프로시저,함수) 생성</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2026 09 18</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -214,7 +178,42 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>2026 09 26</t>
+    <t>2025 09 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025 09 19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025 09 26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025 09 18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025 10 04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RDG 프로그래밍</t>
+  </si>
+  <si>
+    <t>SQL, Procedure</t>
+  </si>
+  <si>
+    <t>SSE</t>
+  </si>
+  <si>
+    <t>DBMS에 성능 수치화</t>
+  </si>
+  <si>
+    <t>데이터 바인딩</t>
+  </si>
+  <si>
+    <t>프로시저 Test 및 수정</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -447,6 +446,9 @@
         </ext>
       </extLst>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -455,9 +457,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -821,7 +820,7 @@
   <dimension ref="A1:L50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -838,16 +837,16 @@
   <sheetData>
     <row r="1" spans="1:12" ht="17.5" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="17"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E3" s="6" t="s">
@@ -917,7 +916,7 @@
       <c r="K5" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L5" s="8" t="s">
         <v>26</v>
       </c>
     </row>
@@ -965,7 +964,7 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" s="8" t="s">
         <v>30</v>
@@ -982,18 +981,18 @@
         <v>12</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="8" t="s">
         <v>39</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="34" x14ac:dyDescent="0.45">
@@ -1001,23 +1000,25 @@
         <v>21</v>
       </c>
       <c r="E9" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="H9" s="4"/>
-      <c r="I9" s="17" t="s">
-        <v>44</v>
+      <c r="I9" s="14" t="s">
+        <v>35</v>
       </c>
       <c r="J9" s="4"/>
       <c r="K9" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="L9" s="8"/>
+        <v>37</v>
+      </c>
+      <c r="L9" s="8" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E10" s="12" t="b">
@@ -1027,16 +1028,16 @@
         <v>21</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="5" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.45">
@@ -1044,26 +1045,28 @@
         <v>0</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
       <c r="J11" s="4"/>
-      <c r="K11" s="5"/>
-      <c r="L11" s="5"/>
+      <c r="K11" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L11" s="8"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="E12" s="12" t="b">
         <v>0</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -1076,10 +1079,10 @@
         <v>0</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
@@ -1092,10 +1095,10 @@
         <v>0</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
@@ -1108,10 +1111,10 @@
         <v>0</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -1123,8 +1126,12 @@
       <c r="E16" s="12" t="b">
         <v>0</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="F16" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>41</v>
+      </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>

</xml_diff>